<commit_message>
Testing path with simx cosim with simulink
</commit_message>
<xml_diff>
--- a/Simulink/Motor_pos.xlsx
+++ b/Simulink/Motor_pos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffeom/Documents/UBC_ELEC/ELEC 391/Main/391_MotoGuzzi/Simulink/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\Documents\ELEC 391\Main\391_MotoGuzzi\Simulink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14873A9C-DA2D-8A42-82BB-55594EA49E67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924F28C3-C2C5-4207-98C6-DE11B3B9D06B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="1380" windowWidth="21800" windowHeight="13100" xr2:uid="{21B0741C-DE49-485B-BE28-83C36ADAE2B0}"/>
+    <workbookView xWindow="465" yWindow="2422" windowWidth="16200" windowHeight="9398" xr2:uid="{21B0741C-DE49-485B-BE28-83C36ADAE2B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,167 +382,167 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8855145B-CAF7-46C9-A3C4-2B3EA4DD37A9}">
   <dimension ref="A1:D331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="A322" sqref="A322:D331"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0.1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>0.2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>0.3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>0.4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>0.5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>0.6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>0.7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D8">
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>0.8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>0.9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1.1000000000000001</v>
       </c>
@@ -556,7 +556,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1.2</v>
       </c>
@@ -570,7 +570,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1.3</v>
       </c>
@@ -584,7 +584,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1.4</v>
       </c>
@@ -598,7 +598,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1.5</v>
       </c>
@@ -612,7 +612,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1.6</v>
       </c>
@@ -626,7 +626,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1.7</v>
       </c>
@@ -640,7 +640,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1.8</v>
       </c>
@@ -654,7 +654,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1.9</v>
       </c>
@@ -668,7 +668,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2</v>
       </c>
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>2.1</v>
       </c>
@@ -696,7 +696,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2.2000000000000002</v>
       </c>
@@ -710,7 +710,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>2.2999999999999998</v>
       </c>
@@ -724,7 +724,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2.4</v>
       </c>
@@ -738,7 +738,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>2.5</v>
       </c>
@@ -752,7 +752,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>2.6</v>
       </c>
@@ -766,7 +766,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>2.7</v>
       </c>
@@ -780,7 +780,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>2.8</v>
       </c>
@@ -794,7 +794,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>2.9</v>
       </c>
@@ -808,7 +808,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>3</v>
       </c>
@@ -822,7 +822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>3.1</v>
       </c>
@@ -830,13 +830,13 @@
         <v>-10</v>
       </c>
       <c r="C32">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>3.1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>3.2</v>
       </c>
@@ -844,13 +844,13 @@
         <v>-10</v>
       </c>
       <c r="C33">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D33">
         <v>3.2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>3.3</v>
       </c>
@@ -858,13 +858,13 @@
         <v>-10</v>
       </c>
       <c r="C34">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D34">
         <v>3.3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>3.4</v>
       </c>
@@ -872,13 +872,13 @@
         <v>-10</v>
       </c>
       <c r="C35">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D35">
         <v>3.4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>3.5</v>
       </c>
@@ -886,13 +886,13 @@
         <v>-10</v>
       </c>
       <c r="C36">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D36">
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>3.6</v>
       </c>
@@ -900,13 +900,13 @@
         <v>-10</v>
       </c>
       <c r="C37">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D37">
         <v>3.6</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>3.7</v>
       </c>
@@ -914,13 +914,13 @@
         <v>-10</v>
       </c>
       <c r="C38">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D38">
         <v>3.7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>3.8</v>
       </c>
@@ -928,13 +928,13 @@
         <v>-10</v>
       </c>
       <c r="C39">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D39">
         <v>3.8</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>3.9</v>
       </c>
@@ -942,13 +942,13 @@
         <v>-10</v>
       </c>
       <c r="C40">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D40">
         <v>3.9</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>4</v>
       </c>
@@ -956,13 +956,13 @@
         <v>-10</v>
       </c>
       <c r="C41">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D41">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>4.0999999999999996</v>
       </c>
@@ -976,7 +976,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>4.2</v>
       </c>
@@ -990,7 +990,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>4.3</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>4.4000000000000004</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>4.5</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>4.5999999999999996</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>4.7</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>4.8</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>4.9000000000000004</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>5</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>5.0999999999999996</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>5.2</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>5.3</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>5.4</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>5.5</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>5.6</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>5.7</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>5.8</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>5.9</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>6</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>6.1</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>6.2</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>6.3</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>6.4</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>6.5</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>6.6</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>6.7</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>6.8</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>6.9</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>7</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>7.1</v>
       </c>
@@ -1390,13 +1390,13 @@
         <v>-10</v>
       </c>
       <c r="C72">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D72">
         <v>7.1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>7.2</v>
       </c>
@@ -1404,13 +1404,13 @@
         <v>-10</v>
       </c>
       <c r="C73">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D73">
         <v>7.2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>7.3</v>
       </c>
@@ -1418,13 +1418,13 @@
         <v>-10</v>
       </c>
       <c r="C74">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D74">
         <v>7.3</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>7.4</v>
       </c>
@@ -1432,13 +1432,13 @@
         <v>-10</v>
       </c>
       <c r="C75">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D75">
         <v>7.4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>7.5</v>
       </c>
@@ -1446,13 +1446,13 @@
         <v>-10</v>
       </c>
       <c r="C76">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D76">
         <v>7.5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>7.6</v>
       </c>
@@ -1460,13 +1460,13 @@
         <v>-10</v>
       </c>
       <c r="C77">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D77">
         <v>7.6</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>7.7</v>
       </c>
@@ -1474,13 +1474,13 @@
         <v>-10</v>
       </c>
       <c r="C78">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D78">
         <v>7.7</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>7.8</v>
       </c>
@@ -1488,13 +1488,13 @@
         <v>-10</v>
       </c>
       <c r="C79">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D79">
         <v>7.8</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>7.9</v>
       </c>
@@ -1502,13 +1502,13 @@
         <v>-10</v>
       </c>
       <c r="C80">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D80">
         <v>7.9</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>8</v>
       </c>
@@ -1516,13 +1516,13 @@
         <v>-10</v>
       </c>
       <c r="C81">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D81">
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>8.1</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>8.1999999999999993</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>8.3000000000000007</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>8.4</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>8.5</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>8.6</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>8.6999999999999993</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>8.8000000000000007</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>8.9</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>9</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>9.1</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>9.1999999999999993</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>9.3000000000000007</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>9.4</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>9.5</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>9.6</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>9.6999999999999993</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>9.8000000000000007</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>9.9</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>10</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>10.1</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>10.199999999999999</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>10.3</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>10.4</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>10.5</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>10.6</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>10.7</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>10.8</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>10.9</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>11</v>
       </c>
@@ -1942,12 +1942,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>11.1</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C112">
         <v>30</v>
@@ -1956,12 +1956,12 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>11.2</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C113">
         <v>30</v>
@@ -1970,12 +1970,12 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>11.3</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C114">
         <v>30</v>
@@ -1984,12 +1984,12 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>11.4</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C115">
         <v>30</v>
@@ -1998,12 +1998,12 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>11.5</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C116">
         <v>30</v>
@@ -2012,12 +2012,12 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>11.6</v>
       </c>
       <c r="B117">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C117">
         <v>30</v>
@@ -2026,12 +2026,12 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>11.7</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C118">
         <v>30</v>
@@ -2040,12 +2040,12 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>11.8</v>
       </c>
       <c r="B119">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C119">
         <v>30</v>
@@ -2054,12 +2054,12 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>11.9</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C120">
         <v>30</v>
@@ -2068,12 +2068,12 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>12</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C121">
         <v>30</v>
@@ -2082,7 +2082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>12.1</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>12.2</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>12.3</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>12.4</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>12.5</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>12.6</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>12.7</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>12.8</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>12.9</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>13</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>13.1</v>
       </c>
@@ -2230,13 +2230,13 @@
         <v>0</v>
       </c>
       <c r="C132">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D132">
         <v>13.1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>13.2</v>
       </c>
@@ -2244,13 +2244,13 @@
         <v>0</v>
       </c>
       <c r="C133">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D133">
         <v>13.2</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>13.3</v>
       </c>
@@ -2258,13 +2258,13 @@
         <v>0</v>
       </c>
       <c r="C134">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D134">
         <v>13.3</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>13.4</v>
       </c>
@@ -2272,13 +2272,13 @@
         <v>0</v>
       </c>
       <c r="C135">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D135">
         <v>13.4</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>13.5</v>
       </c>
@@ -2286,13 +2286,13 @@
         <v>0</v>
       </c>
       <c r="C136">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D136">
         <v>13.5</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>13.6</v>
       </c>
@@ -2300,13 +2300,13 @@
         <v>0</v>
       </c>
       <c r="C137">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D137">
         <v>13.6</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>13.7</v>
       </c>
@@ -2314,13 +2314,13 @@
         <v>0</v>
       </c>
       <c r="C138">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D138">
         <v>13.7</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>13.8</v>
       </c>
@@ -2328,13 +2328,13 @@
         <v>0</v>
       </c>
       <c r="C139">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D139">
         <v>13.8</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>13.9</v>
       </c>
@@ -2342,13 +2342,13 @@
         <v>0</v>
       </c>
       <c r="C140">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D140">
         <v>13.9</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>14</v>
       </c>
@@ -2356,13 +2356,13 @@
         <v>0</v>
       </c>
       <c r="C141">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D141">
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>14.1</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>14.2</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>14.3</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>14.4</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>14.5</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>14.6</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>14.7</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>14.8</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>14.9</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>15</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>15.1</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>15.2</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>15.3</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>15.4</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>15.5</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>15.6</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>15.7</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>15.8</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>15.9</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>16</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>16.100000000000001</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>16.2</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>16.3</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>16.399999999999999</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>16.5</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>16.600000000000001</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>16.7</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>16.8</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>16.899999999999999</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>17</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>17.100000000000001</v>
       </c>
@@ -2790,13 +2790,13 @@
         <v>0</v>
       </c>
       <c r="C172">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D172">
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>17.2</v>
       </c>
@@ -2804,13 +2804,13 @@
         <v>0</v>
       </c>
       <c r="C173">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D173">
         <v>17.2</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>17.3</v>
       </c>
@@ -2818,13 +2818,13 @@
         <v>0</v>
       </c>
       <c r="C174">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D174">
         <v>17.3</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>17.399999999999999</v>
       </c>
@@ -2832,13 +2832,13 @@
         <v>0</v>
       </c>
       <c r="C175">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D175">
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>17.5</v>
       </c>
@@ -2846,13 +2846,13 @@
         <v>0</v>
       </c>
       <c r="C176">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D176">
         <v>17.5</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>17.600000000000001</v>
       </c>
@@ -2860,13 +2860,13 @@
         <v>0</v>
       </c>
       <c r="C177">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D177">
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>17.7</v>
       </c>
@@ -2874,13 +2874,13 @@
         <v>0</v>
       </c>
       <c r="C178">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D178">
         <v>17.7</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>17.8</v>
       </c>
@@ -2888,13 +2888,13 @@
         <v>0</v>
       </c>
       <c r="C179">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D179">
         <v>17.8</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>17.899999999999999</v>
       </c>
@@ -2902,13 +2902,13 @@
         <v>0</v>
       </c>
       <c r="C180">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D180">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>18</v>
       </c>
@@ -2916,13 +2916,13 @@
         <v>0</v>
       </c>
       <c r="C181">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D181">
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>18.100000000000001</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>18.2</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>18.3</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>18.399999999999999</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>18.5</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>18.600000000000001</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>18.7</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>18.8</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>18.899999999999999</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>19</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>19.100000000000001</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>19.2</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>19.3</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>19.399999999999999</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>19.5</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>19.600000000000001</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>19.7</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>19.8</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>19.899999999999999</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>20</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>20.100000000000001</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>20.2</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>20.3</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>20.399999999999999</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>20.5</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>20.6</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>20.7</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>20.8</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>20.9</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>21</v>
       </c>
@@ -3342,12 +3342,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>21.1</v>
       </c>
       <c r="B212">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C212">
         <v>30</v>
@@ -3356,12 +3356,12 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>21.2</v>
       </c>
       <c r="B213">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C213">
         <v>30</v>
@@ -3370,12 +3370,12 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>21.3</v>
       </c>
       <c r="B214">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C214">
         <v>30</v>
@@ -3384,12 +3384,12 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>21.4</v>
       </c>
       <c r="B215">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C215">
         <v>30</v>
@@ -3398,12 +3398,12 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>21.5</v>
       </c>
       <c r="B216">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C216">
         <v>30</v>
@@ -3412,12 +3412,12 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>21.6</v>
       </c>
       <c r="B217">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C217">
         <v>30</v>
@@ -3426,12 +3426,12 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>21.7</v>
       </c>
       <c r="B218">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C218">
         <v>30</v>
@@ -3440,12 +3440,12 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>21.8</v>
       </c>
       <c r="B219">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C219">
         <v>30</v>
@@ -3454,12 +3454,12 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>21.9</v>
       </c>
       <c r="B220">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C220">
         <v>30</v>
@@ -3468,12 +3468,12 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>22</v>
       </c>
       <c r="B221">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C221">
         <v>30</v>
@@ -3482,7 +3482,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>22.1</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>22.2</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>22.3</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>22.4</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>22.5</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>22.6</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>22.7</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>22.8</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>22.9</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>23</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>23.1</v>
       </c>
@@ -3630,13 +3630,13 @@
         <v>10</v>
       </c>
       <c r="C232">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D232">
         <v>23.1</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>23.2</v>
       </c>
@@ -3644,13 +3644,13 @@
         <v>10</v>
       </c>
       <c r="C233">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D233">
         <v>23.2</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>23.3</v>
       </c>
@@ -3658,13 +3658,13 @@
         <v>10</v>
       </c>
       <c r="C234">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D234">
         <v>23.3</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>23.4</v>
       </c>
@@ -3672,13 +3672,13 @@
         <v>10</v>
       </c>
       <c r="C235">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D235">
         <v>23.4</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>23.5</v>
       </c>
@@ -3686,13 +3686,13 @@
         <v>10</v>
       </c>
       <c r="C236">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D236">
         <v>23.5</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>23.6</v>
       </c>
@@ -3700,13 +3700,13 @@
         <v>10</v>
       </c>
       <c r="C237">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D237">
         <v>23.6</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>23.7</v>
       </c>
@@ -3714,13 +3714,13 @@
         <v>10</v>
       </c>
       <c r="C238">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D238">
         <v>23.7</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>23.8</v>
       </c>
@@ -3728,13 +3728,13 @@
         <v>10</v>
       </c>
       <c r="C239">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D239">
         <v>23.8</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>23.9</v>
       </c>
@@ -3742,13 +3742,13 @@
         <v>10</v>
       </c>
       <c r="C240">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D240">
         <v>23.9</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>24</v>
       </c>
@@ -3756,13 +3756,13 @@
         <v>10</v>
       </c>
       <c r="C241">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D241">
         <v>24</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>24.1</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>24.2</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>24.3</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>24.4</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>24.5</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>24.6</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>24.7</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>24.8</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>24.9</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>25</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>25.1</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A253">
         <v>25.1999999999999</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>25.1999999999999</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A254">
         <v>25.3</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A255">
         <v>25.399999999999899</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>25.399999999999899</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A256">
         <v>25.499999999999901</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>25.499999999999901</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A257">
         <v>25.599999999999898</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>25.599999999999898</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A258">
         <v>25.6999999999999</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>25.6999999999999</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A259">
         <v>25.799999999999901</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>25.799999999999901</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A260">
         <v>25.899999999999899</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>25.899999999999899</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A261">
         <v>25.999999999999901</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>25.999999999999901</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A262">
         <v>26.099999999999898</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>26.099999999999898</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A263">
         <v>26.1999999999999</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>26.1999999999999</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A264">
         <v>26.299999999999901</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>26.299999999999901</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A265">
         <v>26.399999999999899</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>26.399999999999899</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A266">
         <v>26.499999999999901</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>26.499999999999901</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A267">
         <v>26.599999999999898</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>26.599999999999898</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A268">
         <v>26.6999999999999</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>26.6999999999999</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A269">
         <v>26.799999999999901</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>26.799999999999901</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A270">
         <v>26.899999999999899</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>26.899999999999899</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A271">
         <v>26.999999999999901</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>26.999999999999901</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A272">
         <v>27.099999999999898</v>
       </c>
@@ -4190,13 +4190,13 @@
         <v>10</v>
       </c>
       <c r="C272">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D272">
         <v>27.099999999999898</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A273">
         <v>27.1999999999999</v>
       </c>
@@ -4204,13 +4204,13 @@
         <v>10</v>
       </c>
       <c r="C273">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D273">
         <v>27.1999999999999</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A274">
         <v>27.299999999999901</v>
       </c>
@@ -4218,13 +4218,13 @@
         <v>10</v>
       </c>
       <c r="C274">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D274">
         <v>27.299999999999901</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A275">
         <v>27.399999999999899</v>
       </c>
@@ -4232,13 +4232,13 @@
         <v>10</v>
       </c>
       <c r="C275">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D275">
         <v>27.399999999999899</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A276">
         <v>27.499999999999901</v>
       </c>
@@ -4246,13 +4246,13 @@
         <v>10</v>
       </c>
       <c r="C276">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D276">
         <v>27.499999999999901</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A277">
         <v>27.599999999999898</v>
       </c>
@@ -4260,13 +4260,13 @@
         <v>10</v>
       </c>
       <c r="C277">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D277">
         <v>27.599999999999898</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A278">
         <v>27.6999999999999</v>
       </c>
@@ -4274,13 +4274,13 @@
         <v>10</v>
       </c>
       <c r="C278">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D278">
         <v>27.6999999999999</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A279">
         <v>27.799999999999901</v>
       </c>
@@ -4288,13 +4288,13 @@
         <v>10</v>
       </c>
       <c r="C279">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D279">
         <v>27.799999999999901</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A280">
         <v>27.899999999999899</v>
       </c>
@@ -4302,13 +4302,13 @@
         <v>10</v>
       </c>
       <c r="C280">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D280">
         <v>27.899999999999899</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A281">
         <v>27.999999999999901</v>
       </c>
@@ -4316,13 +4316,13 @@
         <v>10</v>
       </c>
       <c r="C281">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D281">
         <v>27.999999999999901</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A282">
         <v>28.099999999999898</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>28.099999999999898</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A283">
         <v>28.1999999999999</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>28.1999999999999</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A284">
         <v>28.299999999999901</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>28.299999999999901</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A285">
         <v>28.399999999999899</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>28.399999999999899</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A286">
         <v>28.499999999999901</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>28.499999999999901</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A287">
         <v>28.599999999999898</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>28.599999999999898</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A288">
         <v>28.6999999999999</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>28.6999999999999</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A289">
         <v>28.799999999999901</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>28.799999999999901</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A290">
         <v>28.899999999999899</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>28.899999999999899</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A291">
         <v>28.999999999999901</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>28.999999999999901</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A292">
         <v>29.099999999999898</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>29.099999999999898</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A293">
         <v>29.1999999999999</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>29.1999999999999</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A294">
         <v>29.299999999999901</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>29.299999999999901</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A295">
         <v>29.399999999999899</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>29.399999999999899</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A296">
         <v>29.499999999999901</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>29.499999999999901</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A297">
         <v>29.599999999999898</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>29.599999999999898</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A298">
         <v>29.6999999999999</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>29.6999999999999</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A299">
         <v>29.799999999999901</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>29.799999999999901</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A300">
         <v>29.8999999999998</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>29.8999999999998</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A301">
         <v>29.999999999999901</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>29.999999999999901</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A302">
         <v>30.099999999999799</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>30.099999999999799</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A303">
         <v>30.1999999999998</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>30.1999999999998</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A304">
         <v>30.299999999999802</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>30.299999999999802</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A305">
         <v>30.3999999999998</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>30.3999999999998</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A306">
         <v>30.499999999999801</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>30.499999999999801</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A307">
         <v>30.599999999999799</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>30.599999999999799</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A308">
         <v>30.6999999999998</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>30.6999999999998</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A309">
         <v>30.799999999999802</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>30.799999999999802</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A310">
         <v>30.8999999999998</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>30.8999999999998</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A311">
         <v>30.999999999999801</v>
       </c>
@@ -4742,281 +4742,281 @@
         <v>30.999999999999801</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A312">
         <v>31.099999999999799</v>
       </c>
       <c r="B312">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C312">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D312">
         <v>31.099999999999799</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A313">
         <v>31.1999999999998</v>
       </c>
       <c r="B313">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C313">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D313">
         <v>31.1999999999998</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A314">
         <v>31.299999999999802</v>
       </c>
       <c r="B314">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C314">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D314">
         <v>31.299999999999802</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A315">
         <v>31.3999999999998</v>
       </c>
       <c r="B315">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C315">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D315">
         <v>31.3999999999998</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A316">
         <v>31.499999999999801</v>
       </c>
       <c r="B316">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C316">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D316">
         <v>31.499999999999801</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A317">
         <v>31.599999999999799</v>
       </c>
       <c r="B317">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C317">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D317">
         <v>31.599999999999799</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A318">
         <v>31.6999999999998</v>
       </c>
       <c r="B318">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C318">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D318">
         <v>31.6999999999998</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A319">
         <v>31.799999999999802</v>
       </c>
       <c r="B319">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C319">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D319">
         <v>31.799999999999802</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A320">
         <v>31.8999999999998</v>
       </c>
       <c r="B320">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C320">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D320">
         <v>31.8999999999998</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A321">
         <v>31.999999999999801</v>
       </c>
       <c r="B321">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C321">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D321">
         <v>31.999999999999801</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A322">
         <v>32.099999999999802</v>
       </c>
       <c r="B322">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C322">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D322">
         <v>32.099999999999802</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A323">
         <v>32.199999999999797</v>
       </c>
       <c r="B323">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C323">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D323">
         <v>32.199999999999797</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A324">
         <v>32.299999999999798</v>
       </c>
       <c r="B324">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C324">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D324">
         <v>32.299999999999798</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A325">
         <v>32.3999999999998</v>
       </c>
       <c r="B325">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C325">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D325">
         <v>32.3999999999998</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A326">
         <v>32.499999999999801</v>
       </c>
       <c r="B326">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C326">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D326">
         <v>32.499999999999801</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A327">
         <v>32.599999999999802</v>
       </c>
       <c r="B327">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C327">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D327">
         <v>32.599999999999802</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A328">
         <v>32.699999999999797</v>
       </c>
       <c r="B328">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C328">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D328">
         <v>32.699999999999797</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A329">
         <v>32.799999999999798</v>
       </c>
       <c r="B329">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C329">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D329">
         <v>32.799999999999798</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A330">
         <v>32.8999999999998</v>
       </c>
       <c r="B330">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C330">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D330">
         <v>32.8999999999998</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A331">
         <v>32.999999999999801</v>
       </c>
       <c r="B331">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C331">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D331">
         <v>32.999999999999801</v>

</xml_diff>